<commit_message>
add logs for admin report
</commit_message>
<xml_diff>
--- a/go-api/book1.xlsx
+++ b/go-api/book1.xlsx
@@ -95,6 +95,24 @@
     <t>Test Product 4</t>
   </si>
   <si>
+    <t>20240818113507</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Product 1: 220x500; Test Product 4: 200x1200; </t>
+  </si>
+  <si>
+    <t>20240818113523</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Product 1: 9x500; Test Product 3: 10x1200; </t>
+  </si>
+  <si>
+    <t>20240818113556</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Product 2: 2x1500; </t>
+  </si>
+  <si>
     <t>20240818113344</t>
   </si>
   <si>
@@ -119,24 +137,6 @@
     <t xml:space="preserve">Test Product 1: 1x500; </t>
   </si>
   <si>
-    <t>20240818113507</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Product 1: 220x500; Test Product 4: 200x1200; </t>
-  </si>
-  <si>
-    <t>20240818113523</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Product 1: 9x500; Test Product 3: 10x1200; </t>
-  </si>
-  <si>
-    <t>20240818113556</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Product 2: 2x1500; </t>
-  </si>
-  <si>
     <t>20240818113617</t>
   </si>
   <si>
@@ -152,18 +152,45 @@
     <t>NLJ7RT61SV</t>
   </si>
   <si>
+    <t>20240818181008</t>
+  </si>
+  <si>
+    <t>254708374149</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Product 1: 100x500; Test Product 3: 3x1200; Test Product 2: 1x1500; </t>
+  </si>
+  <si>
+    <t>MPESA</t>
+  </si>
+  <si>
+    <t>20240818181022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Product 1: 30x500; </t>
+  </si>
+  <si>
+    <t>20240818184535</t>
+  </si>
+  <si>
+    <t>087878787</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Product 3: 2x1200; Test Product 4: 10x1200; </t>
+  </si>
+  <si>
+    <t>By Admin</t>
+  </si>
+  <si>
+    <t>Test Product 2</t>
+  </si>
+  <si>
     <t>20240818180820</t>
   </si>
   <si>
-    <t>254708374149</t>
-  </si>
-  <si>
     <t xml:space="preserve">Test Product 1: 21x500; Test Product 2: 2x1500; Test Product 4: 10x1200; </t>
   </si>
   <si>
-    <t>MPESA</t>
-  </si>
-  <si>
     <t>20240818180858</t>
   </si>
   <si>
@@ -177,33 +204,6 @@
   </si>
   <si>
     <t xml:space="preserve">Test Product 1: 1x500; Test Product 2: 1x1500; </t>
-  </si>
-  <si>
-    <t>By Admin</t>
-  </si>
-  <si>
-    <t>Test Product 2</t>
-  </si>
-  <si>
-    <t>20240818181008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Product 1: 100x500; Test Product 3: 3x1200; Test Product 2: 1x1500; </t>
-  </si>
-  <si>
-    <t>20240818181022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Product 1: 30x500; </t>
-  </si>
-  <si>
-    <t>20240818184535</t>
-  </si>
-  <si>
-    <t>087878787</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Product 3: 2x1200; Test Product 4: 10x1200; </t>
   </si>
   <si>
     <t>20240818181106</t>
@@ -709,10 +709,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C2" s="3">
         <v>139300</v>
@@ -724,13 +724,13 @@
         <v>43</v>
       </c>
       <c r="G2" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="H2" t="s">
         <v>45</v>
       </c>
       <c r="I2" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="J2" s="3">
         <v>25500</v>
@@ -750,10 +750,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C3" s="3">
         <v>77700</v>
@@ -765,13 +765,13 @@
         <v>43</v>
       </c>
       <c r="G3" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="H3" t="s">
         <v>45</v>
       </c>
       <c r="I3" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="J3" s="3">
         <v>50000</v>
@@ -791,10 +791,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C4" s="3">
         <v>251000</v>
@@ -806,13 +806,13 @@
         <v>43</v>
       </c>
       <c r="G4" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="H4" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="I4" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="J4" s="3">
         <v>2000</v>
@@ -832,10 +832,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C5" s="3">
         <v>500</v>
@@ -915,10 +915,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C2" s="3">
         <v>350000</v>
@@ -930,13 +930,13 @@
         <v>43</v>
       </c>
       <c r="G2" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="H2" t="s">
         <v>45</v>
       </c>
       <c r="I2" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="J2" s="3">
         <v>55100</v>
@@ -956,10 +956,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C3" s="3">
         <v>16500</v>
@@ -971,13 +971,13 @@
         <v>43</v>
       </c>
       <c r="G3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="H3" t="s">
         <v>45</v>
       </c>
       <c r="I3" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="J3" s="3">
         <v>15000</v>
@@ -997,10 +997,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C4" s="3">
         <v>3000</v>
@@ -1012,13 +1012,13 @@
         <v>43</v>
       </c>
       <c r="G4" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="H4" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="I4" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="J4" s="3">
         <v>14400</v>

</xml_diff>